<commit_message>
9 gestures completely integrated.
Finger 1-5, Swipes right and left, rotation clockwise and counter clockwise implemented succesfully with feedback.
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="113">
   <si>
     <t>Sprint</t>
   </si>
@@ -115,12 +115,21 @@
     <t>Jyothish</t>
   </si>
   <si>
+    <t>PS-1.8</t>
+  </si>
+  <si>
     <t>Integrate FreeRTOS into the project.</t>
   </si>
   <si>
+    <t>PS-1.9</t>
+  </si>
+  <si>
     <t>Create initialization task and start the scheduler.</t>
   </si>
   <si>
+    <t>PS-1.10</t>
+  </si>
+  <si>
     <t>Debug print framework</t>
   </si>
   <si>
@@ -173,15 +182,6 @@
   </si>
   <si>
     <t>Configure LWIP for DHCP address acquisition.</t>
-  </si>
-  <si>
-    <t>DRV-4.3</t>
-  </si>
-  <si>
-    <t>Implement a basic PING test to verify network connectivity.</t>
-  </si>
-  <si>
-    <t>Debugging check.</t>
   </si>
   <si>
     <t>APP-1.1</t>
@@ -892,6 +892,9 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="8">
+        <v>1.0</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -901,17 +904,22 @@
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
+      <c r="I7" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
@@ -933,10 +941,15 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
@@ -950,10 +963,15 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -964,10 +982,17 @@
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D11" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -979,20 +1004,22 @@
         <v>2.0</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="8">
         <v>1.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
@@ -1015,13 +1042,13 @@
         <v>1.0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>33</v>
@@ -1032,21 +1059,25 @@
       <c r="G13" s="4">
         <v>1.0</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="3">
+        <v>0.0</v>
+      </c>
       <c r="I13" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="8"/>
+      <c r="A14" s="8">
+        <v>1.0</v>
+      </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>33</v>
@@ -1062,7 +1093,7 @@
         <v>24</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -1070,13 +1101,13 @@
         <v>1.0</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
@@ -1088,69 +1119,77 @@
         <v>1.5</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="9" t="s">
-        <v>24</v>
+      <c r="I15" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="8">
+        <v>1.0</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1.5</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="8">
+        <v>1.0</v>
+      </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.0</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="2"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="B19" s="4" t="s">
@@ -2520,7 +2559,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F29">
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I15">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I17">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E35">

</xml_diff>

<commit_message>
Debug framewrok partially completed and backlog updated
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -1154,7 +1154,9 @@
       <c r="G16" s="3">
         <v>1.5</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="3">
+        <v>0.0</v>
+      </c>
       <c r="I16" s="9" t="s">
         <v>15</v>
       </c>

</xml_diff>